<commit_message>
pruebas SGCM modulo de ayudas
</commit_message>
<xml_diff>
--- a/PDRMYE/17 REPORTES DE ACTIVIDADES/IRIS CECILIA LECHUGA ARTEAGA/Estimaciones Plataformas.xlsx
+++ b/PDRMYE/17 REPORTES DE ACTIVIDADES/IRIS CECILIA LECHUGA ARTEAGA/Estimaciones Plataformas.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="126">
   <si>
     <t xml:space="preserve">al </t>
   </si>
@@ -400,6 +400,9 @@
   </si>
   <si>
     <t>Accesos</t>
+  </si>
+  <si>
+    <t>doc elec</t>
   </si>
 </sst>
 </file>
@@ -937,11 +940,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E13" sqref="E13"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,7 +999,7 @@
       </c>
       <c r="D4" s="2">
         <f>SUM(D6:D21)</f>
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="F4" t="s">
         <v>2</v>
@@ -1035,7 +1038,7 @@
       </c>
       <c r="C6" s="11"/>
       <c r="D6" s="24">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s">
         <v>6</v>
@@ -1067,7 +1070,7 @@
         <v>115</v>
       </c>
       <c r="D8" s="1">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1078,7 +1081,7 @@
         <v>113</v>
       </c>
       <c r="D9" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1089,7 +1092,7 @@
         <v>116</v>
       </c>
       <c r="D10" s="1">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1097,7 +1100,7 @@
         <v>122</v>
       </c>
       <c r="D11" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1105,7 +1108,15 @@
         <v>124</v>
       </c>
       <c r="D12" s="1">
-        <v>9</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>125</v>
+      </c>
+      <c r="D13" s="1">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>